<commit_message>
Corrected Cap Part Number on BOM
</commit_message>
<xml_diff>
--- a/Electronics/DueShield_BOM.xlsx
+++ b/Electronics/DueShield_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LOCull.STRYKERCORP\Documents\MaslowDue\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB87F92-47CB-4D39-9317-2230D2ECF6D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F0E5CD7-6CF4-4A48-B5AA-50257DDFD39B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="9255" xr2:uid="{0D1909E2-E7BC-4443-9712-339F892941C5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Description</t>
   </si>
@@ -146,9 +146,6 @@
     <t>CAPACITOR, 1uF 50V</t>
   </si>
   <si>
-    <t>CAPACITOR, 10nF, 50V</t>
-  </si>
-  <si>
     <t>CC0805ZRY5V9BB104</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>C0805C100J5GACTU</t>
-  </si>
-  <si>
     <t>CL21F105ZBFNNNE</t>
   </si>
   <si>
@@ -207,6 +201,15 @@
   </si>
   <si>
     <t>Mfg Part Number</t>
+  </si>
+  <si>
+    <t>581-08055C103J</t>
+  </si>
+  <si>
+    <t>MOUSER</t>
+  </si>
+  <si>
+    <t>CAPACITOR, 0.01uF, 50V</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +250,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -443,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -497,6 +506,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -869,7 +884,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,10 +900,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>
@@ -905,13 +920,13 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>4</v>
@@ -925,10 +940,10 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -945,10 +960,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>37</v>
@@ -964,14 +979,14 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
+      <c r="A5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -988,10 +1003,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
@@ -1003,10 +1018,10 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
@@ -1023,10 +1038,10 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
@@ -1043,10 +1058,10 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -1063,13 +1078,13 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
@@ -1083,13 +1098,13 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>23</v>
@@ -1103,13 +1118,13 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>24</v>
@@ -1126,7 +1141,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -1143,13 +1158,13 @@
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
@@ -1166,7 +1181,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Updated P/N on EEPROM for proper package style
</commit_message>
<xml_diff>
--- a/Electronics/DueShield_BOM.xlsx
+++ b/Electronics/DueShield_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LOCull.STRYKERCORP\Documents\MaslowDue\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F0E5CD7-6CF4-4A48-B5AA-50257DDFD39B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAC5261-66BA-4585-917B-D9E9EFC75357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="9255" xr2:uid="{0D1909E2-E7BC-4443-9712-339F892941C5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -125,9 +125,6 @@
     <t>SMA</t>
   </si>
   <si>
-    <t>24LC256T-I/SNCT</t>
-  </si>
-  <si>
     <t>EEPROM, 32K, SOIC</t>
   </si>
   <si>
@@ -210,6 +207,12 @@
   </si>
   <si>
     <t>CAPACITOR, 0.01uF, 50V</t>
+  </si>
+  <si>
+    <t>24LC256T-I/SM</t>
+  </si>
+  <si>
+    <t>updated 4/16/2019</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -508,10 +511,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -884,7 +890,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,10 +906,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>
@@ -920,13 +926,13 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>4</v>
@@ -940,13 +946,13 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -960,13 +966,13 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -980,13 +986,13 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="C5" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -1000,13 +1006,13 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
@@ -1018,10 +1024,10 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
@@ -1038,10 +1044,10 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
@@ -1058,10 +1064,10 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -1078,13 +1084,13 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
@@ -1098,13 +1104,13 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>23</v>
@@ -1118,13 +1124,13 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>24</v>
@@ -1137,14 +1143,14 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
@@ -1158,13 +1164,13 @@
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
@@ -1178,13 +1184,13 @@
     </row>
     <row r="15" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>29</v>
@@ -1194,6 +1200,11 @@
       </c>
       <c r="F15" s="12">
         <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>